<commit_message>
Add another vkey proposal table.
</commit_message>
<xml_diff>
--- a/Docs/Main Engine/Tables/Provisional Virtual Key to Keyboard Mapping Table.xlsx
+++ b/Docs/Main Engine/Tables/Provisional Virtual Key to Keyboard Mapping Table.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\dev\independent\leek\Docs\Main Engine\Tables\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="36" windowWidth="12420" windowHeight="5040"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="133">
   <si>
     <t>0x00</t>
   </si>
@@ -400,13 +405,28 @@
   </si>
   <si>
     <t>APPS</t>
+  </si>
+  <si>
+    <t>Proposal 4</t>
+  </si>
+  <si>
+    <t>EQUAL</t>
+  </si>
+  <si>
+    <t>0/8</t>
+  </si>
+  <si>
+    <t>1/9</t>
+  </si>
+  <si>
+    <t>Even more is ASCII-contiguous, though not necessarily enough that it's noticeable.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,7 +593,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -599,6 +619,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -608,6 +631,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -654,7 +685,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -686,9 +717,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -720,6 +769,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -895,33 +962,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" topLeftCell="F56" workbookViewId="0">
+      <selection activeCell="K61" sqref="K61:K76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" customWidth="1"/>
-    <col min="11" max="11" width="45.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.7890625" customWidth="1"/>
+    <col min="2" max="2" width="10.3125" customWidth="1"/>
+    <col min="5" max="5" width="10.5234375" customWidth="1"/>
+    <col min="9" max="9" width="10.7890625" customWidth="1"/>
+    <col min="11" max="11" width="45.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B3">
         <v>0</v>
       </c>
@@ -953,7 +1020,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -989,7 +1056,7 @@
       </c>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1023,7 +1090,7 @@
       </c>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1057,7 +1124,7 @@
       </c>
       <c r="O6" s="13"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1087,7 +1154,7 @@
       </c>
       <c r="K7" s="22"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1120,7 +1187,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1150,7 +1217,7 @@
       </c>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1180,7 +1247,7 @@
       </c>
       <c r="K10" s="22"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1210,7 +1277,7 @@
       </c>
       <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1240,7 +1307,7 @@
       </c>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1270,7 +1337,7 @@
       </c>
       <c r="K13" s="22"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1300,7 +1367,7 @@
       </c>
       <c r="K14" s="22"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1330,7 +1397,7 @@
       </c>
       <c r="K15" s="22"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1358,7 +1425,7 @@
       <c r="I16" s="5"/>
       <c r="K16" s="22"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1372,7 +1439,7 @@
       <c r="I17" s="5"/>
       <c r="K17" s="22"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1386,7 +1453,7 @@
       <c r="I18" s="5"/>
       <c r="K18" s="22"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1400,12 +1467,12 @@
       <c r="I19" s="8"/>
       <c r="K19" s="22"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B22">
         <v>0</v>
       </c>
@@ -1434,7 +1501,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1466,7 +1533,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1496,7 +1563,7 @@
       </c>
       <c r="K24" s="22"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -1526,7 +1593,7 @@
       </c>
       <c r="K25" s="22"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1556,7 +1623,7 @@
       </c>
       <c r="K26" s="22"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1586,7 +1653,7 @@
       </c>
       <c r="K27" s="22"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1616,7 +1683,7 @@
       </c>
       <c r="K28" s="22"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1646,7 +1713,7 @@
       </c>
       <c r="K29" s="22"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1676,7 +1743,7 @@
       </c>
       <c r="K30" s="22"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1706,7 +1773,7 @@
       </c>
       <c r="K31" s="22"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1736,7 +1803,7 @@
       </c>
       <c r="K32" s="22"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1766,7 +1833,7 @@
       </c>
       <c r="K33" s="22"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -1796,7 +1863,7 @@
       </c>
       <c r="K34" s="22"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -1824,7 +1891,7 @@
       <c r="I35" s="5"/>
       <c r="K35" s="22"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -1838,7 +1905,7 @@
       <c r="I36" s="5"/>
       <c r="K36" s="22"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1852,7 +1919,7 @@
       <c r="I37" s="5"/>
       <c r="K37" s="22"/>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -1866,12 +1933,12 @@
       <c r="I38" s="8"/>
       <c r="K38" s="22"/>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B41">
         <v>0</v>
       </c>
@@ -1900,7 +1967,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -1932,7 +1999,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -1962,7 +2029,7 @@
       </c>
       <c r="K43" s="22"/>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -1982,7 +2049,7 @@
       <c r="I44" s="5"/>
       <c r="K44" s="22"/>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -2012,7 +2079,7 @@
       </c>
       <c r="K45" s="22"/>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -2038,7 +2105,7 @@
       <c r="I46" s="5"/>
       <c r="K46" s="22"/>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -2068,7 +2135,7 @@
       </c>
       <c r="K47" s="22"/>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -2096,7 +2163,7 @@
       <c r="I48" s="5"/>
       <c r="K48" s="22"/>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -2126,7 +2193,7 @@
       </c>
       <c r="K49" s="22"/>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -2144,7 +2211,7 @@
       <c r="I50" s="5"/>
       <c r="K50" s="22"/>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -2174,7 +2241,7 @@
       </c>
       <c r="K51" s="22"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -2204,7 +2271,7 @@
       </c>
       <c r="K52" s="22"/>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -2234,7 +2301,7 @@
       </c>
       <c r="K53" s="22"/>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -2252,7 +2319,7 @@
       <c r="I54" s="5"/>
       <c r="K54" s="22"/>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -2282,7 +2349,7 @@
       </c>
       <c r="K55" s="22"/>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -2312,7 +2379,7 @@
       </c>
       <c r="K56" s="22"/>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -2330,36 +2397,463 @@
       <c r="I57" s="7"/>
       <c r="K57" s="22"/>
     </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B60" t="s">
+        <v>130</v>
+      </c>
+      <c r="C60" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="D60" t="s">
+        <v>121</v>
+      </c>
+      <c r="E60" t="s">
+        <v>122</v>
+      </c>
+      <c r="F60" t="s">
+        <v>123</v>
+      </c>
+      <c r="G60" t="s">
+        <v>124</v>
+      </c>
+      <c r="H60" t="s">
+        <v>125</v>
+      </c>
+      <c r="I60" t="s">
+        <v>126</v>
+      </c>
+      <c r="K60" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="I61" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="K61" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B62" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F62" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="I62" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="K62" s="22"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G63" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I63" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="K63" s="22"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B64" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F64" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G64" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H64" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="I64" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="K64" s="22"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F65" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K65" s="22"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="F66" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K66" s="22"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="9">
+        <v>0</v>
+      </c>
+      <c r="C67" s="10">
+        <v>1</v>
+      </c>
+      <c r="D67" s="10">
+        <v>2</v>
+      </c>
+      <c r="E67" s="10">
+        <v>3</v>
+      </c>
+      <c r="F67" s="10">
+        <v>4</v>
+      </c>
+      <c r="G67" s="10">
+        <v>5</v>
+      </c>
+      <c r="H67" s="10">
+        <v>6</v>
+      </c>
+      <c r="I67" s="11">
+        <v>7</v>
+      </c>
+      <c r="K67" s="22"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B68" s="9">
+        <v>8</v>
+      </c>
+      <c r="C68" s="10">
+        <v>9</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G68" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="K68" s="22"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G69" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H69" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K69" s="22"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B70" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G70" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H70" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I70" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K70" s="22"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I71" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="K71" s="22"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B72" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="K72" s="22"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E73" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F73" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G73" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="H73" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K73" s="22"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B74" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E74" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F74" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G74" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H74" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="I74" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="K74" s="22"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E75" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="K75" s="22"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="K76" s="22"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="K4:K19"/>
     <mergeCell ref="K23:K38"/>
     <mergeCell ref="K42:K57"/>
+    <mergeCell ref="K61:K76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>